<commit_message>
Recorded US deaths now exceed 1958 Flu Pandemic
</commit_message>
<xml_diff>
--- a/Indonesian COVID-19 Infection Projections.xlsx
+++ b/Indonesian COVID-19 Infection Projections.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Aus COVID-19 Projections\Aus-COVID-19-Projections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730987E7-4092-4E4C-A04C-C25DC329D061}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0034BC7-7BC7-4A8D-9240-860866CD374C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{744C986A-0D24-487A-A5C2-8E2494A78887}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="214">
   <si>
     <t>By Age</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>Tourism sites allowed to reopen</t>
+  </si>
+  <si>
+    <t>The official death rate of children to COVID-19 in Indonesia is 2.1% with 28 deaths of children recorded, but it is suspected that the actual number is in the hundreds with 380 deaths of people under 18 with severe COVID-19 symptoms but not testing positive and probably the highest rate of child death due to COVID-19 in the world.  Achmad Yurianto, a senior health ministry official, described Indonesian children as being caught in a "devil's circle" — a cycle of malnutrition and anaemia that increased their vulnerability to the coronavirus.  He compared malnourished children to weak structures that "crumble after an earthquake".</t>
   </si>
 </sst>
 </file>
@@ -1441,6 +1444,8 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1465,8 +1470,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Heading" xfId="3" xr:uid="{DB9EF5E1-A693-41C3-82C7-CA90563DBB00}"/>
@@ -1831,46 +1834,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1980,46 +1983,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2129,46 +2132,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3322,7 +3325,7 @@
                   <c:v>1883</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="#,##0">
-                  <c:v>1923</c:v>
+                  <c:v>2276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11967,7 +11970,7 @@
                   <c:v>1883</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="#,##0">
-                  <c:v>1923</c:v>
+                  <c:v>2276</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12296,46 +12299,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12436,46 +12439,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12579,46 +12582,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12716,46 +12719,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13123,46 +13126,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13272,46 +13275,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13421,46 +13424,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13838,46 +13841,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13978,46 +13981,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14121,46 +14124,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14258,46 +14261,46 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>43952.54217789352</c:v>
+                  <c:v>43959.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43955.54217789352</c:v>
+                  <c:v>43962.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43958.54217789352</c:v>
+                  <c:v>43965.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43961.54217789352</c:v>
+                  <c:v>43968.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43964.54217789352</c:v>
+                  <c:v>43971.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43967.54217789352</c:v>
+                  <c:v>43974.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43970.54217789352</c:v>
+                  <c:v>43977.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43973.54217789352</c:v>
+                  <c:v>43980.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43976.54217789352</c:v>
+                  <c:v>43983.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43979.54217789352</c:v>
+                  <c:v>43986.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43982.54217789352</c:v>
+                  <c:v>43989.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43985.54217789352</c:v>
+                  <c:v>43992.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43988.54217789352</c:v>
+                  <c:v>43995.842825925924</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43991.54217789352</c:v>
+                  <c:v>43998.842825925924</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -33837,167 +33840,167 @@
       </c>
       <c r="B26" s="85">
         <f t="shared" ref="B26:G26" ca="1" si="0">C26-1</f>
-        <v>43952.54217789352</v>
+        <v>43959.842825925924</v>
       </c>
       <c r="C26" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>43953.54217789352</v>
+        <v>43960.842825925924</v>
       </c>
       <c r="D26" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>43954.54217789352</v>
+        <v>43961.842825925924</v>
       </c>
       <c r="E26" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>43955.54217789352</v>
+        <v>43962.842825925924</v>
       </c>
       <c r="F26" s="86">
         <f t="shared" ca="1" si="0"/>
-        <v>43956.54217789352</v>
+        <v>43963.842825925924</v>
       </c>
       <c r="G26" s="87">
         <f t="shared" ca="1" si="0"/>
-        <v>43957.54217789352</v>
+        <v>43964.842825925924</v>
       </c>
       <c r="H26" s="86">
         <f t="shared" ref="H26:U26" ca="1" si="1">I26-1</f>
-        <v>43958.54217789352</v>
+        <v>43965.842825925924</v>
       </c>
       <c r="I26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43959.54217789352</v>
+        <v>43966.842825925924</v>
       </c>
       <c r="J26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43960.54217789352</v>
+        <v>43967.842825925924</v>
       </c>
       <c r="K26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43961.54217789352</v>
+        <v>43968.842825925924</v>
       </c>
       <c r="L26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43962.54217789352</v>
+        <v>43969.842825925924</v>
       </c>
       <c r="M26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43963.54217789352</v>
+        <v>43970.842825925924</v>
       </c>
       <c r="N26" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43964.54217789352</v>
+        <v>43971.842825925924</v>
       </c>
       <c r="O26" s="85">
         <f t="shared" ca="1" si="1"/>
-        <v>43965.54217789352</v>
+        <v>43972.842825925924</v>
       </c>
       <c r="P26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43966.54217789352</v>
+        <v>43973.842825925924</v>
       </c>
       <c r="Q26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43967.54217789352</v>
+        <v>43974.842825925924</v>
       </c>
       <c r="R26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43968.54217789352</v>
+        <v>43975.842825925924</v>
       </c>
       <c r="S26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43969.54217789352</v>
+        <v>43976.842825925924</v>
       </c>
       <c r="T26" s="86">
         <f t="shared" ca="1" si="1"/>
-        <v>43970.54217789352</v>
+        <v>43977.842825925924</v>
       </c>
       <c r="U26" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43971.54217789352</v>
+        <v>43978.842825925924</v>
       </c>
       <c r="V26" s="85">
         <f t="shared" ref="V26:AN26" ca="1" si="2">W26-1</f>
-        <v>43972.54217789352</v>
+        <v>43979.842825925924</v>
       </c>
       <c r="W26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43973.54217789352</v>
+        <v>43980.842825925924</v>
       </c>
       <c r="X26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43974.54217789352</v>
+        <v>43981.842825925924</v>
       </c>
       <c r="Y26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43975.54217789352</v>
+        <v>43982.842825925924</v>
       </c>
       <c r="Z26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43976.54217789352</v>
+        <v>43983.842825925924</v>
       </c>
       <c r="AA26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43977.54217789352</v>
+        <v>43984.842825925924</v>
       </c>
       <c r="AB26" s="87">
         <f t="shared" ca="1" si="2"/>
-        <v>43978.54217789352</v>
+        <v>43985.842825925924</v>
       </c>
       <c r="AC26" s="85">
         <f t="shared" ca="1" si="2"/>
-        <v>43979.54217789352</v>
+        <v>43986.842825925924</v>
       </c>
       <c r="AD26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43980.54217789352</v>
+        <v>43987.842825925924</v>
       </c>
       <c r="AE26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43981.54217789352</v>
+        <v>43988.842825925924</v>
       </c>
       <c r="AF26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43982.54217789352</v>
+        <v>43989.842825925924</v>
       </c>
       <c r="AG26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43983.54217789352</v>
+        <v>43990.842825925924</v>
       </c>
       <c r="AH26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43984.54217789352</v>
+        <v>43991.842825925924</v>
       </c>
       <c r="AI26" s="87">
         <f t="shared" ca="1" si="2"/>
-        <v>43985.54217789352</v>
+        <v>43992.842825925924</v>
       </c>
       <c r="AJ26" s="85">
         <f t="shared" ca="1" si="2"/>
-        <v>43986.54217789352</v>
+        <v>43993.842825925924</v>
       </c>
       <c r="AK26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43987.54217789352</v>
+        <v>43994.842825925924</v>
       </c>
       <c r="AL26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43988.54217789352</v>
+        <v>43995.842825925924</v>
       </c>
       <c r="AM26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43989.54217789352</v>
+        <v>43996.842825925924</v>
       </c>
       <c r="AN26" s="86">
         <f t="shared" ca="1" si="2"/>
-        <v>43990.54217789352</v>
+        <v>43997.842825925924</v>
       </c>
       <c r="AO26" s="86">
         <f ca="1">AP26-1</f>
-        <v>43991.54217789352</v>
+        <v>43998.842825925924</v>
       </c>
       <c r="AP26" s="107">
         <f ca="1">NOW()</f>
-        <v>43992.54217789352</v>
+        <v>43999.842825925924</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.25">
@@ -34132,59 +34135,59 @@
       <c r="A28" s="131" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="290" t="s">
+      <c r="B28" s="292" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="291"/>
-      <c r="D28" s="291"/>
-      <c r="E28" s="291"/>
-      <c r="F28" s="291"/>
-      <c r="G28" s="292"/>
-      <c r="H28" s="296" t="s">
+      <c r="C28" s="293"/>
+      <c r="D28" s="293"/>
+      <c r="E28" s="293"/>
+      <c r="F28" s="293"/>
+      <c r="G28" s="294"/>
+      <c r="H28" s="298" t="s">
         <v>55</v>
       </c>
-      <c r="I28" s="296"/>
-      <c r="J28" s="296"/>
-      <c r="K28" s="296"/>
-      <c r="L28" s="296"/>
-      <c r="M28" s="296"/>
-      <c r="N28" s="297"/>
-      <c r="O28" s="295" t="s">
+      <c r="I28" s="298"/>
+      <c r="J28" s="298"/>
+      <c r="K28" s="298"/>
+      <c r="L28" s="298"/>
+      <c r="M28" s="298"/>
+      <c r="N28" s="299"/>
+      <c r="O28" s="297" t="s">
         <v>56</v>
       </c>
-      <c r="P28" s="296"/>
-      <c r="Q28" s="296"/>
-      <c r="R28" s="296"/>
-      <c r="S28" s="296"/>
-      <c r="T28" s="296"/>
-      <c r="U28" s="297"/>
-      <c r="V28" s="295" t="s">
+      <c r="P28" s="298"/>
+      <c r="Q28" s="298"/>
+      <c r="R28" s="298"/>
+      <c r="S28" s="298"/>
+      <c r="T28" s="298"/>
+      <c r="U28" s="299"/>
+      <c r="V28" s="297" t="s">
         <v>57</v>
       </c>
-      <c r="W28" s="296"/>
-      <c r="X28" s="296"/>
-      <c r="Y28" s="296"/>
-      <c r="Z28" s="296"/>
-      <c r="AA28" s="296"/>
-      <c r="AB28" s="297"/>
-      <c r="AC28" s="295" t="s">
+      <c r="W28" s="298"/>
+      <c r="X28" s="298"/>
+      <c r="Y28" s="298"/>
+      <c r="Z28" s="298"/>
+      <c r="AA28" s="298"/>
+      <c r="AB28" s="299"/>
+      <c r="AC28" s="297" t="s">
         <v>58</v>
       </c>
-      <c r="AD28" s="296"/>
-      <c r="AE28" s="296"/>
-      <c r="AF28" s="296"/>
-      <c r="AG28" s="296"/>
-      <c r="AH28" s="296"/>
-      <c r="AI28" s="297"/>
-      <c r="AJ28" s="295" t="s">
+      <c r="AD28" s="298"/>
+      <c r="AE28" s="298"/>
+      <c r="AF28" s="298"/>
+      <c r="AG28" s="298"/>
+      <c r="AH28" s="298"/>
+      <c r="AI28" s="299"/>
+      <c r="AJ28" s="297" t="s">
         <v>59</v>
       </c>
-      <c r="AK28" s="296"/>
-      <c r="AL28" s="296"/>
-      <c r="AM28" s="296"/>
-      <c r="AN28" s="296"/>
-      <c r="AO28" s="296"/>
-      <c r="AP28" s="297"/>
+      <c r="AK28" s="298"/>
+      <c r="AL28" s="298"/>
+      <c r="AM28" s="298"/>
+      <c r="AN28" s="298"/>
+      <c r="AO28" s="298"/>
+      <c r="AP28" s="299"/>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B29" s="51" t="s">
@@ -34195,43 +34198,43 @@
       <c r="E29" s="92"/>
       <c r="F29" s="92"/>
       <c r="G29" s="93"/>
-      <c r="H29" s="293" t="s">
+      <c r="H29" s="295" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="293"/>
-      <c r="J29" s="293"/>
-      <c r="K29" s="293"/>
-      <c r="L29" s="293"/>
-      <c r="M29" s="293"/>
-      <c r="N29" s="293"/>
-      <c r="O29" s="293"/>
-      <c r="P29" s="293"/>
-      <c r="Q29" s="293"/>
-      <c r="R29" s="293"/>
-      <c r="S29" s="293"/>
-      <c r="T29" s="293"/>
-      <c r="U29" s="293"/>
-      <c r="V29" s="293"/>
-      <c r="W29" s="293"/>
-      <c r="X29" s="293"/>
-      <c r="Y29" s="293"/>
-      <c r="Z29" s="293"/>
-      <c r="AA29" s="293"/>
-      <c r="AB29" s="293"/>
-      <c r="AC29" s="293"/>
-      <c r="AD29" s="293"/>
-      <c r="AE29" s="293"/>
-      <c r="AF29" s="293"/>
-      <c r="AG29" s="293"/>
-      <c r="AH29" s="293"/>
-      <c r="AI29" s="293"/>
-      <c r="AJ29" s="293"/>
-      <c r="AK29" s="293"/>
-      <c r="AL29" s="293"/>
-      <c r="AM29" s="293"/>
-      <c r="AN29" s="293"/>
-      <c r="AO29" s="293"/>
-      <c r="AP29" s="294"/>
+      <c r="I29" s="295"/>
+      <c r="J29" s="295"/>
+      <c r="K29" s="295"/>
+      <c r="L29" s="295"/>
+      <c r="M29" s="295"/>
+      <c r="N29" s="295"/>
+      <c r="O29" s="295"/>
+      <c r="P29" s="295"/>
+      <c r="Q29" s="295"/>
+      <c r="R29" s="295"/>
+      <c r="S29" s="295"/>
+      <c r="T29" s="295"/>
+      <c r="U29" s="295"/>
+      <c r="V29" s="295"/>
+      <c r="W29" s="295"/>
+      <c r="X29" s="295"/>
+      <c r="Y29" s="295"/>
+      <c r="Z29" s="295"/>
+      <c r="AA29" s="295"/>
+      <c r="AB29" s="295"/>
+      <c r="AC29" s="295"/>
+      <c r="AD29" s="295"/>
+      <c r="AE29" s="295"/>
+      <c r="AF29" s="295"/>
+      <c r="AG29" s="295"/>
+      <c r="AH29" s="295"/>
+      <c r="AI29" s="295"/>
+      <c r="AJ29" s="295"/>
+      <c r="AK29" s="295"/>
+      <c r="AL29" s="295"/>
+      <c r="AM29" s="295"/>
+      <c r="AN29" s="295"/>
+      <c r="AO29" s="295"/>
+      <c r="AP29" s="296"/>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B31" s="57" t="s">
@@ -34900,13 +34903,12 @@
       <c r="N18" s="155"/>
       <c r="O18" s="47"/>
       <c r="P18" s="69"/>
-      <c r="T18" s="266">
-        <v>43997</v>
-      </c>
-      <c r="U18" s="267" t="s">
-        <v>211</v>
-      </c>
-      <c r="V18" s="69"/>
+      <c r="T18" s="205">
+        <v>43994</v>
+      </c>
+      <c r="U18" t="s">
+        <v>213</v>
+      </c>
       <c r="W18" s="276"/>
       <c r="X18" s="155"/>
       <c r="Y18" s="69"/>
@@ -34939,10 +34941,10 @@
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
       <c r="T19" s="266">
-        <v>44002</v>
+        <v>43997</v>
       </c>
       <c r="U19" s="267" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="V19" s="69"/>
       <c r="W19" s="69"/>
@@ -34974,7 +34976,13 @@
       <c r="N20" s="69"/>
       <c r="O20" s="230"/>
       <c r="P20" s="16"/>
-      <c r="V20" s="155"/>
+      <c r="T20" s="266">
+        <v>44002</v>
+      </c>
+      <c r="U20" s="267" t="s">
+        <v>212</v>
+      </c>
+      <c r="V20" s="69"/>
       <c r="W20" s="69"/>
       <c r="X20" s="69"/>
       <c r="Y20" s="155"/>
@@ -38193,8 +38201,8 @@
         <f t="shared" ref="T56" si="62">T53-T57-T55</f>
         <v>10904</v>
       </c>
-      <c r="U56" s="298">
-        <v>11414</v>
+      <c r="U56" s="290">
+        <v>16243</v>
       </c>
       <c r="V56" s="174"/>
       <c r="W56" s="174"/>
@@ -38256,8 +38264,8 @@
       <c r="T57" s="52">
         <v>1883</v>
       </c>
-      <c r="U57" s="299">
-        <v>1923</v>
+      <c r="U57" s="291">
+        <v>2276</v>
       </c>
       <c r="V57" s="175"/>
       <c r="W57" s="175"/>
@@ -42643,7 +42651,7 @@
         <v>117</v>
       </c>
       <c r="C6" s="153">
-        <v>33076</v>
+        <v>41431</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
@@ -42652,7 +42660,7 @@
       </c>
       <c r="C7" s="151">
         <f ca="1">NOW()</f>
-        <v>43992.54217789352</v>
+        <v>43999.842825925924</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -42661,7 +42669,7 @@
       </c>
       <c r="C8" s="152">
         <f ca="1">C7-C5</f>
-        <v>92.542177893519693</v>
+        <v>99.842825925923535</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -42670,7 +42678,7 @@
       </c>
       <c r="C9" s="154">
         <f ca="1">C8/(LOG(C6/C4)/LOG(2))</f>
-        <v>9.2102729341758156</v>
+        <v>9.6255956131301552</v>
       </c>
       <c r="D9" t="s">
         <v>96</v>
@@ -42703,7 +42711,7 @@
       </c>
       <c r="C12" s="159">
         <f>C6/Projections!B17</f>
-        <v>139391.71428571429</v>
+        <v>174602.07142857142</v>
       </c>
     </row>
     <row r="13" spans="2:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
@@ -42712,7 +42720,7 @@
       </c>
       <c r="C13" s="160">
         <f ca="1">(C4/Projections!B17)*(2^(((C7-21)-C5)/C9))</f>
-        <v>28699.193150279509</v>
+        <v>38485.516105321993</v>
       </c>
     </row>
     <row r="14" spans="2:10" s="69" customFormat="1" x14ac:dyDescent="0.25">
@@ -42721,7 +42729,7 @@
       </c>
       <c r="C14" s="143">
         <f ca="1">C12-C13</f>
-        <v>110692.52113543478</v>
+        <v>136116.55532324943</v>
       </c>
       <c r="E14" s="156"/>
       <c r="F14" s="157" t="s">
@@ -42735,7 +42743,7 @@
       </c>
       <c r="C15" s="64">
         <f>C6*Projections!B21</f>
-        <v>26791.56</v>
+        <v>33559.11</v>
       </c>
       <c r="I15" s="150"/>
     </row>
@@ -42745,7 +42753,7 @@
       </c>
       <c r="C16" s="79">
         <f ca="1">(C4*Projections!B21)*(2^(((C7-21)-C5)/C9))</f>
-        <v>5516.0822088842324</v>
+        <v>7397.0466548195163</v>
       </c>
       <c r="I16" s="150"/>
     </row>
@@ -42755,7 +42763,7 @@
       </c>
       <c r="C17" s="79">
         <f ca="1">C15-C16</f>
-        <v>21275.477791115769</v>
+        <v>26162.063345180482</v>
       </c>
       <c r="F17" t="s">
         <v>141</v>
@@ -42768,7 +42776,7 @@
       </c>
       <c r="C18" s="64">
         <f>C6*Projections!B22</f>
-        <v>4630.6400000000003</v>
+        <v>5800.34</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -42777,7 +42785,7 @@
       </c>
       <c r="C19" s="79">
         <f ca="1">(C4*Projections!B22)*(2^(((C7-49)-C5)/C9))</f>
-        <v>115.90906007536512</v>
+        <v>170.22836936943932</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -42786,7 +42794,7 @@
       </c>
       <c r="C20" s="79">
         <f ca="1">C18-C19</f>
-        <v>4514.7309399246351</v>
+        <v>5630.1116306305612</v>
       </c>
       <c r="F20" t="s">
         <v>146</v>
@@ -42798,7 +42806,7 @@
       </c>
       <c r="C21" s="64">
         <f>C6*Projections!B23</f>
-        <v>1653.8000000000002</v>
+        <v>2071.5500000000002</v>
       </c>
       <c r="I21" s="150"/>
     </row>
@@ -42808,7 +42816,7 @@
       </c>
       <c r="C22" s="79">
         <f ca="1">(C4*Projections!B23)*(2^(((C7-49)-C5)/C9))</f>
-        <v>41.396092884058973</v>
+        <v>60.795846203371184</v>
       </c>
       <c r="I22" s="150"/>
     </row>
@@ -42818,7 +42826,7 @@
       </c>
       <c r="C23" s="79">
         <f ca="1">C21-C22</f>
-        <v>1612.4039071159411</v>
+        <v>2010.754153796629</v>
       </c>
       <c r="I23" s="150"/>
     </row>
@@ -42828,7 +42836,7 @@
       </c>
       <c r="C24" s="64">
         <f>C6*Projections!B24</f>
-        <v>1951.4839999999999</v>
+        <v>2444.4290000000001</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -42837,7 +42845,7 @@
       </c>
       <c r="C25" s="61">
         <f ca="1">(C4*Projections!B24)*(2^(((C7-42)-C5)/C9))</f>
-        <v>82.723795196630746</v>
+        <v>118.76084360765965</v>
       </c>
       <c r="F25" t="s">
         <v>152</v>
@@ -42849,7 +42857,7 @@
       </c>
       <c r="C26" s="163">
         <f ca="1">C9*(LOG(C10/C21)/LOG(2))</f>
-        <v>61.058622092389733</v>
+        <v>60.684358999455242</v>
       </c>
       <c r="D26" t="s">
         <v>96</v>
@@ -42864,7 +42872,7 @@
       </c>
       <c r="C27" s="162">
         <f ca="1">C7+C26</f>
-        <v>44053.600799985907</v>
+        <v>44060.527184925377</v>
       </c>
       <c r="F27" t="s">
         <v>154</v>
@@ -42876,7 +42884,7 @@
       </c>
       <c r="C28" s="161">
         <f ca="1">C9*(LOG(C11/C21)/LOG(2))</f>
-        <v>19.852494759126671</v>
+        <v>17.620106579596591</v>
       </c>
       <c r="D28" t="s">
         <v>96</v>
@@ -42888,7 +42896,7 @@
       </c>
       <c r="C29" s="162">
         <f ca="1">C7+C28</f>
-        <v>44012.394672652648</v>
+        <v>44017.462932505521</v>
       </c>
       <c r="F29" t="s">
         <v>154</v>
@@ -42900,7 +42908,7 @@
       </c>
       <c r="C30" s="161">
         <f ca="1">C9*(LOG((C3*0.6)/C12)/LOG(2))</f>
-        <v>93.926107931925898</v>
+        <v>95.033952086727552</v>
       </c>
       <c r="D30" t="s">
         <v>96</v>
@@ -42912,7 +42920,7 @@
       </c>
       <c r="C31" s="162">
         <f ca="1">C7+C30</f>
-        <v>44086.468285825445</v>
+        <v>44094.876778012651</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -42921,7 +42929,7 @@
       </c>
       <c r="C34" s="151">
         <f ca="1">C7+30</f>
-        <v>44022.54217789352</v>
+        <v>44029.842825925924</v>
       </c>
       <c r="F34" t="s">
         <v>167</v>
@@ -42933,7 +42941,7 @@
       </c>
       <c r="C35" s="79">
         <f ca="1">C6*(2^((C34-C7)/C9))</f>
-        <v>316255.18730307918</v>
+        <v>359370.70224697684</v>
       </c>
       <c r="F35" t="s">
         <v>139</v>
@@ -42945,7 +42953,7 @@
       </c>
       <c r="C36" s="79">
         <f ca="1">C35/Projections!B17</f>
-        <v>1332789.7179201194</v>
+        <v>1514490.8166122595</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -42954,7 +42962,7 @@
       </c>
       <c r="C37" s="79">
         <f ca="1">C35*Projections!B21</f>
-        <v>256166.70171549416</v>
+        <v>291090.26882005128</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -42963,7 +42971,7 @@
       </c>
       <c r="C38" s="79">
         <f ca="1">C35*Projections!B22</f>
-        <v>44275.726222431091</v>
+        <v>50311.898314576763</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -42972,7 +42980,7 @@
       </c>
       <c r="C39" s="79">
         <f ca="1">C35*Projections!B23</f>
-        <v>15812.759365153959</v>
+        <v>17968.535112348844</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -42981,7 +42989,7 @@
       </c>
       <c r="C40" s="61">
         <f ca="1">C35*Projections!B24</f>
-        <v>18659.056050881671</v>
+        <v>21202.871432571632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>